<commit_message>
upd: password protect the excels
</commit_message>
<xml_diff>
--- a/assets/compiled_july_2025.xlsx
+++ b/assets/compiled_july_2025.xlsx
@@ -8,16 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\65961\Documents\git_projects\sbf_2025\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70CC3A55-A79D-44E5-8CDC-90AE8C73FE02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2830B460-3076-4F46-8258-2A74DB4C836C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="D26q9QgX6BWVPtiRGcmxCbvYlDOoOd7avoj0OcTrdnDnt8QeX3x7eUg7qimZGv3Y9zfjbko40wNEP+/PmNRqUg==" workbookSaltValue="O1M7+NVQ5n2oP1UcCF7Hfg==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{44DBA47A-370E-4A02-956B-779FF0AF8C99}"/>
   </bookViews>
   <sheets>
-    <sheet name="README" sheetId="13" r:id="rId1"/>
-    <sheet name="2025JULY" sheetId="3" r:id="rId2"/>
+    <sheet name="2025JULY" sheetId="3" r:id="rId1"/>
+    <sheet name="README" sheetId="13" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'2025JULY'!$A$1:$Q$1541</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'2025JULY'!$A$1:$Q$1541</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -1280,7 +1281,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -1329,14 +1330,8 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="24" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -1364,10 +1359,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/richData/rdRichValueTypes.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1750,152 +1741,13 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8DCBD23-B9A3-4234-A643-0378CB8E2923}">
-  <dimension ref="A1:C18"/>
-  <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="112.85546875" customWidth="1"/>
-    <col min="2" max="2" width="5.140625" customWidth="1"/>
-    <col min="3" max="3" width="21.140625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" ht="56.25" x14ac:dyDescent="0.3">
-      <c r="A1" s="35" t="s">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="37" t="s">
-        <v>310</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>311</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A7" s="34" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B8" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B9" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>304</v>
-      </c>
-      <c r="B10" s="39">
-        <v>1</v>
-      </c>
-      <c r="C10" s="40" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B11" s="39">
-        <v>2</v>
-      </c>
-      <c r="C11" s="40" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="38" t="s">
-        <v>305</v>
-      </c>
-      <c r="B12" s="39">
-        <v>3</v>
-      </c>
-      <c r="C12" s="40" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="38" t="s">
-        <v>313</v>
-      </c>
-      <c r="B13" s="39">
-        <v>4</v>
-      </c>
-      <c r="C13" s="40" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="38" t="s">
-        <v>306</v>
-      </c>
-      <c r="B14" s="39">
-        <v>5</v>
-      </c>
-      <c r="C14" s="40" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B15" s="39">
-        <v>6</v>
-      </c>
-      <c r="C15" s="40" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B16" s="39">
-        <v>7</v>
-      </c>
-      <c r="C16" s="40" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" ht="21" x14ac:dyDescent="0.35">
-      <c r="A17" s="36" t="s">
-        <v>307</v>
-      </c>
-      <c r="B17" s="39">
-        <v>8</v>
-      </c>
-      <c r="C17" s="40" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" ht="217.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" t="e" vm="1">
-        <v>#VALUE!</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8098871B-0A0E-451D-B2CD-505BC1892A22}">
   <sheetPr>
     <tabColor rgb="FFFF0000"/>
   </sheetPr>
   <dimension ref="A1:Q1541"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A1522" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B1540" sqref="B1540"/>
     </sheetView>
@@ -1920,53 +1772,53 @@
     <col min="16" max="16" width="12.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="42" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A1" s="42" t="s">
+    <row r="1" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="42" t="s">
+      <c r="B1" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="42" t="s">
+      <c r="C1" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="42" t="s">
+      <c r="D1" t="s">
         <v>21</v>
       </c>
-      <c r="E1" s="42" t="s">
+      <c r="E1" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="42" t="s">
+      <c r="F1" t="s">
         <v>22</v>
       </c>
-      <c r="G1" s="43" t="s">
+      <c r="G1" s="42" t="s">
         <v>84</v>
       </c>
-      <c r="H1" s="44" t="s">
+      <c r="H1" s="43" t="s">
         <v>0</v>
       </c>
-      <c r="I1" s="42" t="s">
+      <c r="I1" t="s">
         <v>23</v>
       </c>
-      <c r="J1" s="42" t="s">
+      <c r="J1" t="s">
         <v>24</v>
       </c>
-      <c r="K1" s="42" t="s">
+      <c r="K1" t="s">
         <v>25</v>
       </c>
-      <c r="L1" s="45" t="s">
+      <c r="L1" s="34" t="s">
         <v>1</v>
       </c>
-      <c r="M1" s="46" t="s">
+      <c r="M1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="N1" s="47" t="s">
+      <c r="N1" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="O1" s="46" t="s">
+      <c r="O1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="P1" s="42" t="s">
+      <c r="P1" t="s">
         <v>314</v>
       </c>
       <c r="Q1" s="41" t="s">
@@ -83596,4 +83448,144 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8DCBD23-B9A3-4234-A643-0378CB8E2923}">
+  <dimension ref="A1:C18"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="112.85546875" customWidth="1"/>
+    <col min="2" max="2" width="5.140625" customWidth="1"/>
+    <col min="3" max="3" width="21.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="56.25" x14ac:dyDescent="0.3">
+      <c r="A1" s="35" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="37" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A7" s="34" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>304</v>
+      </c>
+      <c r="B10" s="39">
+        <v>1</v>
+      </c>
+      <c r="C10" s="40" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B11" s="39">
+        <v>2</v>
+      </c>
+      <c r="C11" s="40" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="38" t="s">
+        <v>305</v>
+      </c>
+      <c r="B12" s="39">
+        <v>3</v>
+      </c>
+      <c r="C12" s="40" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="38" t="s">
+        <v>313</v>
+      </c>
+      <c r="B13" s="39">
+        <v>4</v>
+      </c>
+      <c r="C13" s="40" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="38" t="s">
+        <v>306</v>
+      </c>
+      <c r="B14" s="39">
+        <v>5</v>
+      </c>
+      <c r="C14" s="40" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B15" s="39">
+        <v>6</v>
+      </c>
+      <c r="C15" s="40" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B16" s="39">
+        <v>7</v>
+      </c>
+      <c r="C16" s="40" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+      <c r="A17" s="36" t="s">
+        <v>307</v>
+      </c>
+      <c r="B17" s="39">
+        <v>8</v>
+      </c>
+      <c r="C17" s="40" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="217.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" t="e" vm="1">
+        <v>#VALUE!</v>
+      </c>
+    </row>
+  </sheetData>
+  <sheetProtection algorithmName="SHA-512" hashValue="3q3LeOJqIXlMQ8Ushb2LHrcflSU9GA8eVbn3UYxE5/wSk7TKSuWIUH+OkZjw5YhrUblpoaRz38RFQajG4d6kww==" saltValue="ABL1XFpYSFadpRQH/3873g==" spinCount="100000" sheet="1" formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>